<commit_message>
Final Revision before refactoring
</commit_message>
<xml_diff>
--- a/NurieBoard/WikiDB Requirements.xlsx
+++ b/NurieBoard/WikiDB Requirements.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="위키 데이터베이스 기능 목록표" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>입력값</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,6 +127,122 @@
   </si>
   <si>
     <t>getDocumentFrameList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getDocumentFullData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getDocumentRawData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON reldocIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON frameList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON Parsed Document Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON Raw(Non-parsed) Document Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[관련있는,문서]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docID 문서의 상위/관련 문서 리스트를 가져 옵니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Frame:임시,Frame:틀1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docID 문서의 틀 리스트를 가져옵니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타 시트 참조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타 시트 참조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docID 문서의 파싱된 데이터를 가져 옵니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docID 문서의 데이터를 가져옵니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getFrameData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>frameID, frameTier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"'''이 틀은 임시 틀입니다!'''"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FrameTier등급의 FrameID 틀을 가져옵니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isDocumentExists</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boolean docExists</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문서가 존재하는지/아닌지를 반환합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>testFunction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트 값을 입력합니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -134,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +263,14 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -194,7 +318,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -202,6 +326,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -484,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -590,14 +717,121 @@
       <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>